<commit_message>
se corrigio ejercicios del 20191024
</commit_message>
<xml_diff>
--- a/m1/u1/ejemplos/20191023/ExcelEjercicio4.xlsx
+++ b/m1/u1/ejemplos/20191023/ExcelEjercicio4.xlsx
@@ -89,9 +89,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -124,6 +124,10 @@
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -199,14 +203,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -216,22 +218,26 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -536,7 +542,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -547,321 +553,369 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="1" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="15">
         <v>0.05</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="8" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="13">
         <v>0.02</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="15">
         <v>0.08</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="10" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="14">
         <v>0.03</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="15">
         <v>0.03</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="15">
         <v>0.04</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="8">
         <v>65.150000000000006</v>
       </c>
-      <c r="C11" s="13">
-        <f>B11+B11*$B4</f>
+      <c r="C11" s="8">
+        <f>B11*$B4+B11</f>
         <v>68.407499999999999</v>
       </c>
-      <c r="D11" s="13">
-        <f>C11+C11*$B4</f>
+      <c r="D11" s="8">
+        <f t="shared" ref="D11:E11" si="0">C11*$B4+C11</f>
         <v>71.827875000000006</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="E11" s="8">
+        <f t="shared" si="0"/>
+        <v>75.419268750000001</v>
+      </c>
+      <c r="F11" s="8">
+        <f>SUM(B11:E11)</f>
+        <v>280.80464375000003</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="8">
         <v>44.75</v>
       </c>
-      <c r="C12" s="13">
-        <f t="shared" ref="C12:D14" si="0">B12+B12*$B5</f>
+      <c r="C12" s="8">
+        <f t="shared" ref="C12:E12" si="1">B12*$B5+B12</f>
         <v>48.33</v>
       </c>
-      <c r="D12" s="13">
-        <f t="shared" si="0"/>
+      <c r="D12" s="8">
+        <f t="shared" si="1"/>
         <v>52.196399999999997</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
+      <c r="E12" s="8">
+        <f t="shared" si="1"/>
+        <v>56.372111999999994</v>
+      </c>
+      <c r="F12" s="8">
+        <f t="shared" ref="F12:F14" si="2">SUM(B12:E12)</f>
+        <v>201.64851199999998</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="8">
         <v>83.12</v>
       </c>
-      <c r="C13" s="13">
-        <f t="shared" si="0"/>
+      <c r="C13" s="8">
+        <f t="shared" ref="C13:E13" si="3">B13*$B6+B13</f>
         <v>85.613600000000005</v>
       </c>
-      <c r="D13" s="13">
-        <f t="shared" si="0"/>
+      <c r="D13" s="8">
+        <f t="shared" si="3"/>
         <v>88.18200800000001</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
+      <c r="E13" s="8">
+        <f t="shared" si="3"/>
+        <v>90.827468240000016</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" si="2"/>
+        <v>347.74307624000005</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="8">
         <v>50.35</v>
       </c>
-      <c r="C14" s="13">
-        <f t="shared" si="0"/>
+      <c r="C14" s="8">
+        <f t="shared" ref="C14:E14" si="4">B14*$B7+B14</f>
         <v>52.364000000000004</v>
       </c>
-      <c r="D14" s="13">
-        <f t="shared" si="0"/>
+      <c r="D14" s="8">
+        <f t="shared" si="4"/>
         <v>54.458560000000006</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="E14" s="8">
+        <f t="shared" si="4"/>
+        <v>56.636902400000004</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="2"/>
+        <v>213.8094624</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="9">
         <f>SUM(B11:B14)</f>
         <v>243.37</v>
       </c>
-      <c r="C15" s="14">
-        <f t="shared" ref="C15:F15" si="1">SUM(C11:C14)</f>
+      <c r="C15" s="9">
+        <f t="shared" ref="C15:E15" si="5">SUM(C11:C14)</f>
         <v>254.71510000000001</v>
       </c>
-      <c r="D15" s="14">
-        <f t="shared" si="1"/>
+      <c r="D15" s="9">
+        <f t="shared" si="5"/>
         <v>266.66484300000002</v>
       </c>
-      <c r="E15" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="14">
+      <c r="E15" s="9">
+        <f t="shared" si="5"/>
+        <v>279.25575139</v>
+      </c>
+      <c r="F15" s="9">
         <f>B15+C15+D15+E15</f>
-        <v>764.74994300000003</v>
+        <v>1044.0056943899999</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="8">
         <v>12</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="C16" s="8">
+        <f>B16*$F4+B16</f>
+        <v>12.24</v>
+      </c>
+      <c r="D16" s="8">
+        <f t="shared" ref="D16:E16" si="6">C16*$F4+C16</f>
+        <v>12.4848</v>
+      </c>
+      <c r="E16" s="8">
+        <f t="shared" si="6"/>
+        <v>12.734496</v>
+      </c>
+      <c r="F16" s="8">
+        <f>SUM(B16:E16)</f>
+        <v>49.459296000000002</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="8">
         <v>15.4</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
+      <c r="C17" s="8">
+        <f>B17*$F5+B17</f>
+        <v>15.862</v>
+      </c>
+      <c r="D17" s="8">
+        <f t="shared" ref="D17:E17" si="7">C17*$F5+C17</f>
+        <v>16.337859999999999</v>
+      </c>
+      <c r="E17" s="8">
+        <f t="shared" si="7"/>
+        <v>16.8279958</v>
+      </c>
+      <c r="F17" s="8">
+        <f>SUM(B17:E17)</f>
+        <v>64.427855800000003</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="9">
         <f>SUM(B16:B17)</f>
         <v>27.4</v>
       </c>
-      <c r="C18" s="14">
-        <f t="shared" ref="C18:F18" si="2">SUM(C16:C17)</f>
-        <v>0</v>
-      </c>
-      <c r="D18" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="14">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="C18" s="9">
+        <f t="shared" ref="C18:F18" si="8">SUM(C16:C17)</f>
+        <v>28.102</v>
+      </c>
+      <c r="D18" s="9">
+        <f t="shared" si="8"/>
+        <v>28.822659999999999</v>
+      </c>
+      <c r="E18" s="9">
+        <f t="shared" si="8"/>
+        <v>29.5624918</v>
+      </c>
+      <c r="F18" s="9">
+        <f t="shared" si="8"/>
+        <v>113.8871518</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="10">
         <f>B15-B18</f>
         <v>215.97</v>
       </c>
-      <c r="C19" s="15">
-        <f t="shared" ref="C19:F19" si="3">C15-C18</f>
-        <v>254.71510000000001</v>
-      </c>
-      <c r="D19" s="15">
-        <f t="shared" si="3"/>
-        <v>266.66484300000002</v>
-      </c>
-      <c r="E19" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="15">
-        <f t="shared" si="3"/>
-        <v>764.74994300000003</v>
+      <c r="C19" s="10">
+        <f t="shared" ref="C19:F19" si="9">C15-C18</f>
+        <v>226.6131</v>
+      </c>
+      <c r="D19" s="10">
+        <f t="shared" si="9"/>
+        <v>237.84218300000003</v>
+      </c>
+      <c r="E19" s="10">
+        <f t="shared" si="9"/>
+        <v>249.69325959</v>
+      </c>
+      <c r="F19" s="10">
+        <f t="shared" si="9"/>
+        <v>930.11854258999995</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="15">
+      <c r="B20" s="10">
         <f>B19</f>
         <v>215.97</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="10">
         <f>B20+C19</f>
-        <v>470.68510000000003</v>
-      </c>
-      <c r="D20" s="15">
-        <f t="shared" ref="D20:F20" si="4">C20+D19</f>
-        <v>737.34994300000005</v>
-      </c>
-      <c r="E20" s="15">
-        <f t="shared" si="4"/>
-        <v>737.34994300000005</v>
-      </c>
-      <c r="F20" s="15">
-        <f t="shared" si="4"/>
-        <v>1502.099886</v>
+        <v>442.5831</v>
+      </c>
+      <c r="D20" s="10">
+        <f t="shared" ref="D20:F20" si="10">C20+D19</f>
+        <v>680.42528300000004</v>
+      </c>
+      <c r="E20" s="10">
+        <f t="shared" si="10"/>
+        <v>930.11854259000006</v>
+      </c>
+      <c r="F20" s="10">
+        <f t="shared" si="10"/>
+        <v>1860.2370851800001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>